<commit_message>
correct status detail alcohol + comment computer use
</commit_message>
<xml_diff>
--- a/data_processing_elements-FRA.xlsx
+++ b/data_processing_elements-FRA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlaforme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DF0C80-49AA-4086-9451-A2C1DED60B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51376CF-8180-4E9C-8807-87C1612AF3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="465">
   <si>
     <t>index</t>
   </si>
@@ -1775,6 +1775,9 @@
   </si>
   <si>
     <t>recode(1=0; 2=1; 3=2; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>Wording specifies "daily time spent at home using a computer"</t>
   </si>
 </sst>
 </file>
@@ -2237,10 +2240,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomRight" activeCell="O71" sqref="O71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4450,7 +4453,7 @@
         <v>27</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>49</v>
@@ -5975,7 +5978,9 @@
         <v>412</v>
       </c>
       <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
+      <c r="O73" s="1" t="s">
+        <v>464</v>
+      </c>
       <c r="P73" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Correcting cog_depression, dis_hypercholesteromia DPE + valuetype fruit and vegetable intake
</commit_message>
<xml_diff>
--- a/data_processing_elements-FRA.xlsx
+++ b/data_processing_elements-FRA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51376CF-8180-4E9C-8807-87C1612AF3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A674C7-B2E5-4D3E-9E87-F30DCBDE1940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1389,9 +1389,6 @@
     <t>Depression. Self-reported. Questionnaire item: Has a doctor/physician given you a diagnosis of depression? Response options: no, yes: previously, yes: currently.</t>
   </si>
   <si>
-    <t>recode(1=0; 2=1; 3=1; ELSE=99)</t>
-  </si>
-  <si>
     <t>mci1</t>
   </si>
   <si>
@@ -1778,6 +1775,9 @@
   </si>
   <si>
     <t>Wording specifies "daily time spent at home using a computer"</t>
+  </si>
+  <si>
+    <t>recode(1=NA; 2=1; 3=1; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -1819,7 +1819,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1850,6 +1850,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1863,7 +1869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1898,6 +1904,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2240,10 +2249,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O71" sqref="O71"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2443,7 @@
         <v>36</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -3333,7 +3342,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="9"/>
       <c r="J21" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>335</v>
@@ -3390,7 +3399,7 @@
         <v>98</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>335</v>
@@ -3415,7 +3424,7 @@
         <v>36</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -3515,7 +3524,7 @@
         <v>36</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="T24" s="6" t="s">
         <v>341</v>
@@ -3574,7 +3583,7 @@
         <v>36</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -3631,7 +3640,7 @@
         <v>36</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -3904,7 +3913,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="9"/>
       <c r="J32" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>142</v>
@@ -3953,7 +3962,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="9"/>
       <c r="J33" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>145</v>
@@ -4002,7 +4011,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="9"/>
       <c r="J34" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>147</v>
@@ -4051,10 +4060,10 @@
       <c r="H35" s="1"/>
       <c r="I35" s="9"/>
       <c r="J35" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="K35" s="10" t="s">
         <v>451</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>452</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="9"/>
@@ -4070,7 +4079,7 @@
         <v>36</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
@@ -4100,7 +4109,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="9"/>
       <c r="J36" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>151</v>
@@ -4149,7 +4158,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="9"/>
       <c r="J37" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>153</v>
@@ -4190,7 +4199,7 @@
         <v>157</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>158</v>
@@ -4284,7 +4293,7 @@
         <v>166</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>158</v>
@@ -4536,7 +4545,7 @@
         <v>183</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>359</v>
@@ -4559,7 +4568,7 @@
         <v>43</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
@@ -4743,7 +4752,7 @@
         <v>196</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>368</v>
@@ -4795,10 +4804,10 @@
         <v>196</v>
       </c>
       <c r="J50" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="K50" s="10" t="s">
         <v>437</v>
-      </c>
-      <c r="K50" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>372</v>
@@ -4808,7 +4817,7 @@
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>27</v>
@@ -4820,7 +4829,7 @@
         <v>211</v>
       </c>
       <c r="S50" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
@@ -5033,8 +5042,8 @@
       <c r="R54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S54" s="1" t="s">
-        <v>378</v>
+      <c r="S54" s="14" t="s">
+        <v>464</v>
       </c>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
@@ -5064,7 +5073,7 @@
         <v>196</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>384</v>
@@ -5087,7 +5096,7 @@
         <v>211</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T55" s="6" t="s">
         <v>387</v>
@@ -5119,7 +5128,7 @@
         <v>196</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>384</v>
@@ -5142,7 +5151,7 @@
         <v>211</v>
       </c>
       <c r="S56" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T56" s="6" t="s">
         <v>387</v>
@@ -5174,7 +5183,7 @@
         <v>196</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>384</v>
@@ -5197,7 +5206,7 @@
         <v>211</v>
       </c>
       <c r="S57" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="T57" s="6" t="s">
         <v>387</v>
@@ -5252,7 +5261,7 @@
         <v>43</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>391</v>
+        <v>327</v>
       </c>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
@@ -5505,16 +5514,16 @@
       <c r="H64" s="1"/>
       <c r="I64" s="9"/>
       <c r="J64" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="L64" s="1" t="s">
+      <c r="M64" s="9" t="s">
         <v>394</v>
-      </c>
-      <c r="M64" s="9" t="s">
-        <v>395</v>
       </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -5603,13 +5612,13 @@
         <v>235</v>
       </c>
       <c r="J66" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="K66" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="L66" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>398</v>
       </c>
       <c r="M66" s="9" t="s">
         <v>376</v>
@@ -5656,20 +5665,20 @@
       <c r="H67" s="1"/>
       <c r="I67" s="9"/>
       <c r="J67" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>296</v>
       </c>
       <c r="L67" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M67" s="9" t="s">
         <v>400</v>
-      </c>
-      <c r="M67" s="9" t="s">
-        <v>401</v>
       </c>
       <c r="N67" s="1"/>
       <c r="O67" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="P67" s="1" t="s">
         <v>27</v>
@@ -5681,7 +5690,7 @@
         <v>43</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -5711,16 +5720,16 @@
         <v>241</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>296</v>
       </c>
       <c r="L68" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M68" s="9" t="s">
         <v>400</v>
-      </c>
-      <c r="M68" s="9" t="s">
-        <v>401</v>
       </c>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -5734,7 +5743,7 @@
         <v>43</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -5764,16 +5773,16 @@
         <v>244</v>
       </c>
       <c r="J69" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="K69" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="L69" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="M69" s="9" t="s">
         <v>407</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>408</v>
       </c>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -5817,20 +5826,20 @@
         <v>247</v>
       </c>
       <c r="J70" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="K70" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="M70" s="9" t="s">
         <v>411</v>
-      </c>
-      <c r="M70" s="9" t="s">
-        <v>412</v>
       </c>
       <c r="N70" s="1"/>
       <c r="O70" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P70" s="1" t="s">
         <v>27</v>
@@ -5842,7 +5851,7 @@
         <v>43</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
@@ -5966,20 +5975,20 @@
         <v>255</v>
       </c>
       <c r="J73" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="K73" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="L73" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="M73" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P73" s="1" t="s">
         <v>27</v>
@@ -5991,7 +6000,7 @@
         <v>36</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
@@ -6115,20 +6124,20 @@
       <c r="H76" s="1"/>
       <c r="I76" s="9"/>
       <c r="J76" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="K76" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="K76" s="10" t="s">
+      <c r="L76" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="L76" s="1" t="s">
-        <v>421</v>
-      </c>
       <c r="M76" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N76" s="1"/>
       <c r="O76" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P76" s="1" t="s">
         <v>27</v>
@@ -6140,7 +6149,7 @@
         <v>36</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
@@ -6168,20 +6177,20 @@
         <v>270</v>
       </c>
       <c r="J77" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="K77" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="K77" s="10" t="s">
+      <c r="L77" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>421</v>
-      </c>
       <c r="M77" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P77" s="1" t="s">
         <v>27</v>
@@ -6193,7 +6202,7 @@
         <v>211</v>
       </c>
       <c r="S77" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
@@ -6364,16 +6373,16 @@
         <v>196</v>
       </c>
       <c r="J81" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="K81" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="L81" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="L81" s="1" t="s">
+      <c r="M81" s="9" t="s">
         <v>427</v>
-      </c>
-      <c r="M81" s="9" t="s">
-        <v>428</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -6387,7 +6396,7 @@
         <v>43</v>
       </c>
       <c r="S81" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
@@ -6417,20 +6426,20 @@
         <v>196</v>
       </c>
       <c r="J82" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="K82" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="M82" s="9" t="s">
         <v>432</v>
-      </c>
-      <c r="M82" s="9" t="s">
-        <v>433</v>
       </c>
       <c r="N82" s="1"/>
       <c r="O82" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P82" s="1" t="s">
         <v>27</v>
@@ -6442,7 +6451,7 @@
         <v>43</v>
       </c>
       <c r="S82" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
@@ -6470,7 +6479,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="9"/>
       <c r="J83" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
@@ -6487,7 +6496,7 @@
         <v>36</v>
       </c>
       <c r="S83" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
@@ -6517,7 +6526,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="9"/>
       <c r="J84" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
@@ -6534,7 +6543,7 @@
         <v>36</v>
       </c>
       <c r="S84" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>

</xml_diff>